<commit_message>
Finalized CycleCount App Service
</commit_message>
<xml_diff>
--- a/aspnet-core/src/BishalAgroSeed.DbMigrator/CycleCounts/UpdateCycleCountTemplate.xlsx
+++ b/aspnet-core/src/BishalAgroSeed.DbMigrator/CycleCounts/UpdateCycleCountTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0dfecb421916105a/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\BishalAgroSeed\aspnet-core\src\BishalAgroSeed.DbMigrator\CycleCounts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{5569D82A-1307-4BEC-91DC-0FAE683D3E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFB709A5-D8F8-4955-A7E4-8EFE8BFA9CB5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBB8EFA-35A3-41B1-A9F7-CF744A48FA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AE12EAAB-24CD-44D2-8C95-CF4AC1EDFF0E}"/>
   </bookViews>
@@ -51,6 +51,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -88,9 +91,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,24 +414,24 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.109375" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="33.109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>